<commit_message>
DCDC21V and DCDC3V3 calculus updated. They should be more accurate now.
</commit_message>
<xml_diff>
--- a/Board/_01_Documents_Projet/Power_supplies_calculus.xlsx
+++ b/Board/_01_Documents_Projet/Power_supplies_calculus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badr\Documents\prt-ge-s2-2015-svn\trunk\_01_Documents_Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badr\Documents\prt-ge-s2-2015-svn\trunk\Board\_01_Documents_Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Duty Cycle" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Duty Cycle</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>Ripple target Δil (percentage of max. output current and A)</t>
+  </si>
+  <si>
+    <t>Worst case</t>
+  </si>
+  <si>
+    <t>Voltage dropout accross the internal MOSFET</t>
+  </si>
+  <si>
+    <t>ΔVout (V)</t>
+  </si>
+  <si>
+    <t>In the other way around</t>
   </si>
 </sst>
 </file>
@@ -537,19 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -796,6 +795,19 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -812,9 +824,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1"/>
@@ -823,14 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="3" fillId="2" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
@@ -838,19 +840,48 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -858,12 +889,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,39 +904,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="22" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calcul" xfId="4" builtinId="22"/>
@@ -1512,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,123 +1531,134 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="9"/>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="20"/>
+      <c r="E2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>3.3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>3.3</v>
       </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f>C4/C3</f>
         <v>0.65999999999999992</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E7" s="8" t="s">
+      <c r="F6" s="4">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="6" t="s">
+      <c r="F7" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f>F6*F7</f>
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="22">
+      <c r="F9" s="6">
         <f>(F4+F5)/(F3+F5-F8)</f>
-        <v>0.65999999999999992</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E11" s="23" t="s">
+        <v>0.70035964414158614</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="1">
+      <c r="F11" s="40"/>
+      <c r="G11" s="16">
         <f>(F9-C5)/F9</f>
-        <v>0</v>
+        <v>5.7627027027027024E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1650,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,115 +1680,115 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="13"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="20" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="C9" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="D9" s="11">
         <f>C9*C8</f>
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+        <v>0.17</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="13">
         <v>1600000</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="D10" s="4"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="13">
         <f>1/C10</f>
         <v>6.2500000000000005E-7</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="F11" s="21" t="s">
+      <c r="D11" s="4"/>
+      <c r="F11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="18">
-        <f>('Duty Cycle'!C5*C11)/(2*D9)*('Duty Cycle'!C3-'Duty Cycle'!C4)</f>
-        <v>3.5062500000000001E-6</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="C12" s="14">
+        <f>('Duty Cycle'!F9*C11)/(2*D9)*('Duty Cycle'!C3-'Duty Cycle'!C4)</f>
+        <v>2.1886238879424572E-6</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1785,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,232 +1815,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H1" s="24"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="2:13" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
-      <c r="H3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="38"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="27"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="33"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="38"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="30"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="27"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="38"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="27"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="37"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="38"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="27"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="36"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="37"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="38"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="30"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="27"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="30"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="36"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H10" s="24"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="30"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="36"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <f>'Inductor value'!C8*SQRT('Duty Cycle'!C5*(1-'Duty Cycle'!C5))</f>
-        <v>0.47370877129308048</v>
-      </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="30"/>
+        <f>'Inductor value'!C8*SQRT('Duty Cycle'!F9*(1-'Duty Cycle'!F9))</f>
+        <v>0.45810043985948862</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="2:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="24"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="36"/>
     </row>
     <row r="13" spans="2:13" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H13" s="24"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="33"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="39"/>
     </row>
     <row r="14" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="H14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="38"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="3" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="27"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="38"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="42" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="27"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="43">
+      <c r="J16" s="45">
         <v>0.1</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="4">
         <f>J16*'Duty Cycle'!C4</f>
         <v>0.33</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="38"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="1" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="27"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="44" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="14">
         <f>1/((8*'Inductor value'!C10)*(K16/'Inductor value'!D9-J15))</f>
-        <v>2.3674242424242426E-8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="38"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="38"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="38"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="38"/>
-      <c r="H21" s="24"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="37"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="38"/>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="38"/>
-      <c r="H23" s="24"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="41"/>
-      <c r="H24" s="24"/>
+        <v>4.0246212121212125E-8</v>
+      </c>
+      <c r="K17" s="43"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="27"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="27"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="43"/>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="27"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="13">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="K20" s="43"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="27"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="14">
+        <f>'Inductor value'!D9*(J19+1/(8*'Inductor value'!C10*J20))</f>
+        <v>6.0369318181818191E-4</v>
+      </c>
+      <c r="K21" s="43"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="27"/>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="27"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="28"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="H24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2039,7 +2085,7 @@
   <dimension ref="B13:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,8 +2095,8 @@
         <v>27</v>
       </c>
       <c r="C13" s="1">
-        <f>('Inductor value'!C8)*(1-'Duty Cycle'!C5)</f>
-        <v>0.34000000000000008</v>
+        <f>('Inductor value'!C8)*(1-'Duty Cycle'!F9)</f>
+        <v>0.29964035585841386</v>
       </c>
     </row>
   </sheetData>
@@ -2063,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B15:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2119,7 @@
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="19">
         <v>10000</v>
       </c>
     </row>
@@ -2081,7 +2127,7 @@
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="18">
         <f>(('Duty Cycle'!C4/0.6)-1)*C15</f>
         <v>45000</v>
       </c>

</xml_diff>